<commit_message>
updating code WQCA code and files with high low flow data analysis
</commit_message>
<xml_diff>
--- a/WQCAn/local_WQ.xlsx
+++ b/WQCAn/local_WQ.xlsx
@@ -786,12 +786,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1136,14 +1137,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q282"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B278"/>
+    <sheetView tabSelected="1" topLeftCell="C243" workbookViewId="0">
+      <selection activeCell="E255" sqref="E255:J260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" customWidth="1"/>
+    <col min="5" max="5" width="47.5703125" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
     <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="13.140625" customWidth="1"/>
@@ -10065,8 +10066,8 @@
       <c r="G170" t="s">
         <v>57</v>
       </c>
-      <c r="H170" t="s">
-        <v>55</v>
+      <c r="H170" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="I170">
         <v>42.630273000000003</v>

</xml_diff>